<commit_message>
implementation of Cyl SDDR
</commit_message>
<xml_diff>
--- a/Default Settings/Config.xlsx
+++ b/Default Settings/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.laghi\Documents\GitHub\JADE\Code\Default Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC7CE6E-49B2-4BBD-B207-6352B7D76FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD6F3D8-C818-44C1-B960-64FDF3C5E69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>xsdir Path</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>mcnp6</t>
+  </si>
+  <si>
+    <t>ITER Cylindrical benchmark for SDDR</t>
+  </si>
+  <si>
+    <t>ITER_Cyl_SDDR.i</t>
+  </si>
+  <si>
+    <t>D1S5</t>
   </si>
 </sst>
 </file>
@@ -800,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -999,14 +1008,29 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
+      <c r="A9" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="20">
+        <v>500000000</v>
+      </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
+      <c r="I9" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
@@ -1032,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EEB530-2BB1-44BD-96B5-AB98331CD0CC}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>

</xml_diff>